<commit_message>
duration changing added, 07.02
</commit_message>
<xml_diff>
--- a/testDate.xlsx
+++ b/testDate.xlsx
@@ -1331,7 +1331,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="4" s="7" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
-        <v>10011</v>
+        <v>9984</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>7488</v>
@@ -1410,7 +1410,7 @@
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="str">
         <f aca="false">A3&amp;A4</f>
-        <v>https://app3.reevio.com/editor/10011</v>
+        <v>https://app3.reevio.com/editor/9984</v>
       </c>
       <c r="B5" s="8" t="str">
         <f aca="false">B3&amp;B4</f>
@@ -1427,7 +1427,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>18</v>

</xml_diff>